<commit_message>
Updated data to studies with CompletionDate before 2023
</commit_message>
<xml_diff>
--- a/Data/inputs/20240531_df_results.xlsx
+++ b/Data/inputs/20240531_df_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julien.bacquart\Development\BSO-Inserm-Sante\Data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6929EFAF-B3C8-4DB4-98D7-31B9DF8323FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F8B13C-629B-4C01-8BD7-50E84E6B2888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54C56140-7FA7-4032-8563-70EB33033164}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">df_for_manual_treatment!$B$1:$O$501</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4294,7 +4293,7 @@
   <dimension ref="A1:Q501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q458" sqref="Q458"/>
+      <selection activeCell="K501" sqref="K501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>